<commit_message>
1.Created migrations for all tables. 2. Upload the database design file. @ E:\SALINDA SANDARUWAN\SIBA_Dynamics\SIBA-Inventory-system-Dynamics\Inventory-2k23\Documents\siba_inventory_2k23_database_design.pdf
</commit_message>
<xml_diff>
--- a/Documents/ER_Inventory/Test_Excel.xlsx
+++ b/Documents/ER_Inventory/Test_Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SALINDA SANDARUWAN\SIBA_Dynamics\SIBA-Inventory-system-Dynamics\Inventory-2k23\Documents\ER_Inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C2F5B8-75B6-4DAD-940B-6D393CBCD0E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33EC674-8FDD-451A-89B3-7FDEA4EDF077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{7C6AD97D-0354-4FD0-8E91-EBAC4EC551C4}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="184">
   <si>
     <t>state</t>
   </si>
@@ -616,7 +616,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:mm"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -664,18 +664,12 @@
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -711,19 +705,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -735,9 +723,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -745,23 +730,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1078,11 +1063,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95CA8C8-82BE-40BC-8871-F9C457D45A7D}">
   <dimension ref="A2:T159"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="70" zoomScaleNormal="117" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A148" zoomScale="102" zoomScaleNormal="117" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B157" sqref="B157"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
@@ -1100,7 +1085,7 @@
     <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1108,67 +1093,67 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="31.2" customHeight="1">
-      <c r="C3" s="18" t="s">
+    <row r="3" spans="1:16" s="1" customFormat="1" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="K3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="N3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="O3" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="3" customFormat="1" ht="54.6" customHeight="1">
-      <c r="C4" s="6"/>
-      <c r="D4" s="7" t="s">
+    <row r="4" spans="1:16" s="3" customFormat="1" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="4"/>
+      <c r="D4" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
@@ -1189,7 +1174,7 @@
         <v>33</v>
       </c>
       <c r="J5" s="2"/>
-      <c r="K5" s="8"/>
+      <c r="K5" s="6"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2">
@@ -1199,7 +1184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
@@ -1230,7 +1215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1261,7 +1246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1292,7 +1277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="18.600000000000001" customHeight="1">
+    <row r="9" spans="1:16" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
@@ -1323,7 +1308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1354,7 +1339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
@@ -1385,7 +1370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1399,7 +1384,7 @@
       </c>
       <c r="P14" s="2"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1419,7 +1404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1439,7 +1424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G17" s="2" t="s">
         <v>16</v>
       </c>
@@ -1447,7 +1432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G18" s="2" t="s">
         <v>17</v>
       </c>
@@ -1455,7 +1440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G19" s="2" t="s">
         <v>18</v>
       </c>
@@ -1463,7 +1448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1471,21 +1456,21 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="18.600000000000001" customHeight="1">
-      <c r="C24" s="18" t="s">
+    <row r="24" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C25" s="2" t="s">
         <v>55</v>
       </c>
@@ -1499,7 +1484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C26" s="2" t="s">
         <v>56</v>
       </c>
@@ -1513,7 +1498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C27" s="2" t="s">
         <v>57</v>
       </c>
@@ -1527,7 +1512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C28" s="2" t="s">
         <v>58</v>
       </c>
@@ -1541,7 +1526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C29" s="2" t="s">
         <v>59</v>
       </c>
@@ -1555,7 +1540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C30" s="2" t="s">
         <v>60</v>
       </c>
@@ -1569,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C31" s="2" t="s">
         <v>61</v>
       </c>
@@ -1583,47 +1568,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="1" customFormat="1" ht="28.8">
-      <c r="C35" s="18" t="s">
+    <row r="35" spans="1:12" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C35" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E35" s="19" t="s">
+      <c r="E35" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="F35" s="19" t="s">
+      <c r="F35" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="G35" s="19" t="s">
+      <c r="G35" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="H35" s="20" t="s">
+      <c r="H35" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="I35" s="5" t="s">
+      <c r="I35" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="J35" s="5" t="s">
+      <c r="J35" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="K35" s="14" t="s">
+      <c r="K35" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="L35" s="9" t="s">
+      <c r="L35" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1639,7 +1624,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1651,7 +1636,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" ht="15">
+    <row r="38" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="C38" s="2">
         <v>1234</v>
       </c>
@@ -1674,14 +1659,14 @@
       <c r="J38" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K38" s="11">
+      <c r="K38" s="8">
         <v>45243.737835648149</v>
       </c>
-      <c r="L38" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="15">
+      <c r="L38" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="C39" s="2">
         <v>1235</v>
       </c>
@@ -1704,14 +1689,14 @@
       <c r="J39" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K39" s="11">
+      <c r="K39" s="8">
         <v>45243.737835648149</v>
       </c>
-      <c r="L39" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="15">
+      <c r="L39" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="C40" s="2">
         <v>1236</v>
       </c>
@@ -1734,14 +1719,14 @@
       <c r="J40" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K40" s="11">
+      <c r="K40" s="8">
         <v>45243.737835648149</v>
       </c>
-      <c r="L40" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="15">
+      <c r="L40" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="C41" s="2">
         <v>1237</v>
       </c>
@@ -1764,14 +1749,14 @@
       <c r="J41" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K41" s="11">
+      <c r="K41" s="8">
         <v>45243.737835648149</v>
       </c>
-      <c r="L41" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="15">
+      <c r="L41" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="C42" s="2">
         <v>1238</v>
       </c>
@@ -1794,14 +1779,14 @@
       <c r="J42" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K42" s="11">
+      <c r="K42" s="8">
         <v>45244.737835648149</v>
       </c>
-      <c r="L42" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="15">
+      <c r="L42" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="C43" s="2">
         <v>1239</v>
       </c>
@@ -1824,14 +1809,14 @@
       <c r="J43" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K43" s="11">
+      <c r="K43" s="8">
         <v>45245.737835648149</v>
       </c>
-      <c r="L43" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="15">
+      <c r="L43" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="C44" s="2">
         <v>1240</v>
       </c>
@@ -1854,20 +1839,20 @@
       <c r="J44" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K44" s="11">
+      <c r="K44" s="8">
         <v>45246.737835648149</v>
       </c>
-      <c r="L44" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12">
+      <c r="L44" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D48" s="2" t="s">
         <v>183</v>
       </c>
       <c r="E48" s="2"/>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D49" s="2" t="s">
         <v>78</v>
       </c>
@@ -1875,7 +1860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D50" s="2" t="s">
         <v>79</v>
       </c>
@@ -1883,7 +1868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D51" s="2" t="s">
         <v>148</v>
       </c>
@@ -1891,7 +1876,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="53" spans="1:20">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>4</v>
       </c>
@@ -1899,45 +1884,45 @@
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="1:20" s="1" customFormat="1" ht="43.2">
-      <c r="C54" s="4" t="s">
+    <row r="54" spans="1:20" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C54" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="F54" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="G54" s="5" t="s">
+      <c r="G54" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="H54" s="14" t="s">
+      <c r="H54" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="I54" s="14" t="s">
+      <c r="I54" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="J54" s="5" t="s">
+      <c r="J54" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="K54" s="5" t="s">
+      <c r="K54" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="L54" s="14" t="s">
+      <c r="L54" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="M54" s="14" t="s">
+      <c r="M54" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="N54" s="9" t="s">
+      <c r="N54" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:20">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C55" s="2" t="s">
         <v>80</v>
       </c>
@@ -1961,7 +1946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:20">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C56" s="2" t="s">
         <v>81</v>
       </c>
@@ -1985,7 +1970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:20">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C57" s="2" t="s">
         <v>82</v>
       </c>
@@ -2009,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:20">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C58" s="2" t="s">
         <v>83</v>
       </c>
@@ -2033,7 +2018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:20">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C59" s="2" t="s">
         <v>84</v>
       </c>
@@ -2056,15 +2041,15 @@
       <c r="N59" s="2">
         <v>1</v>
       </c>
-      <c r="T59" s="16"/>
-    </row>
-    <row r="62" spans="1:20">
+      <c r="T59" s="12"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D62" s="2" t="s">
         <v>93</v>
       </c>
       <c r="E62" s="2"/>
     </row>
-    <row r="63" spans="1:20">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D63" s="2" t="s">
         <v>99</v>
       </c>
@@ -2072,7 +2057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:20">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D64" s="2" t="s">
         <v>100</v>
       </c>
@@ -2080,7 +2065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>5</v>
       </c>
@@ -2088,36 +2073,36 @@
         <v>101</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="1" customFormat="1">
-      <c r="C70" s="15" t="s">
+    <row r="70" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C70" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="D70" s="17" t="s">
+      <c r="D70" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E70" s="5" t="s">
+      <c r="E70" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="F70" s="14" t="s">
+      <c r="F70" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="G70" s="5" t="s">
+      <c r="G70" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="H70" s="5" t="s">
+      <c r="H70" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="I70" s="5" t="s">
+      <c r="I70" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="J70" s="5" t="s">
+      <c r="J70" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="K70" s="9" t="s">
+      <c r="K70" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C71" s="2" t="s">
         <v>113</v>
       </c>
@@ -2132,7 +2117,7 @@
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C72" s="2" t="s">
         <v>114</v>
       </c>
@@ -2147,7 +2132,7 @@
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C73" s="2" t="s">
         <v>115</v>
       </c>
@@ -2162,7 +2147,7 @@
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C74" s="2" t="s">
         <v>116</v>
       </c>
@@ -2177,7 +2162,7 @@
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C75" s="2" t="s">
         <v>117</v>
       </c>
@@ -2192,7 +2177,7 @@
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C76" s="2" t="s">
         <v>118</v>
       </c>
@@ -2207,13 +2192,13 @@
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E79" s="2" t="s">
         <v>104</v>
       </c>
       <c r="F79" s="2"/>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E80" s="2" t="s">
         <v>120</v>
       </c>
@@ -2221,7 +2206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E81" s="2" t="s">
         <v>121</v>
       </c>
@@ -2229,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>6</v>
       </c>
@@ -2237,27 +2222,27 @@
         <v>122</v>
       </c>
     </row>
-    <row r="87" spans="1:8" s="1" customFormat="1" ht="28.8">
-      <c r="C87" s="15" t="s">
+    <row r="87" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C87" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="D87" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="E87" s="5" t="s">
+      <c r="E87" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="F87" s="14" t="s">
+      <c r="F87" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="G87" s="5" t="s">
+      <c r="G87" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="H87" s="9" t="s">
+      <c r="H87" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C88" s="2" t="s">
         <v>172</v>
       </c>
@@ -2269,7 +2254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C89" s="2" t="s">
         <v>173</v>
       </c>
@@ -2281,7 +2266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C90" s="2" t="s">
         <v>174</v>
       </c>
@@ -2293,7 +2278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C91" s="2" t="s">
         <v>175</v>
       </c>
@@ -2305,7 +2290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C92" s="2" t="s">
         <v>176</v>
       </c>
@@ -2317,7 +2302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C93" s="2" t="s">
         <v>177</v>
       </c>
@@ -2327,7 +2312,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C94" s="2" t="s">
         <v>178</v>
       </c>
@@ -2337,13 +2322,13 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F96" s="2" t="s">
         <v>104</v>
       </c>
       <c r="G96" s="2"/>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F97" s="2" t="s">
         <v>125</v>
       </c>
@@ -2351,7 +2336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F98" s="2" t="s">
         <v>126</v>
       </c>
@@ -2359,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>7</v>
       </c>
@@ -2367,30 +2352,30 @@
         <v>127</v>
       </c>
     </row>
-    <row r="104" spans="1:9" s="1" customFormat="1" ht="28.8">
-      <c r="C104" s="4" t="s">
+    <row r="104" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C104" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D104" s="4" t="s">
+      <c r="D104" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E104" s="5" t="s">
+      <c r="E104" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="F104" s="5" t="s">
+      <c r="F104" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G104" s="14" t="s">
+      <c r="G104" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="H104" s="5" t="s">
+      <c r="H104" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="I104" s="9" t="s">
+      <c r="I104" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C105" s="2" t="s">
         <v>164</v>
       </c>
@@ -2403,7 +2388,7 @@
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C106" s="2" t="s">
         <v>165</v>
       </c>
@@ -2416,7 +2401,7 @@
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C107" s="2" t="s">
         <v>166</v>
       </c>
@@ -2429,7 +2414,7 @@
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C108" s="2" t="s">
         <v>167</v>
       </c>
@@ -2442,7 +2427,7 @@
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C109" s="2" t="s">
         <v>168</v>
       </c>
@@ -2455,7 +2440,7 @@
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C110" s="2" t="s">
         <v>169</v>
       </c>
@@ -2468,7 +2453,7 @@
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C111" s="2" t="s">
         <v>170</v>
       </c>
@@ -2481,7 +2466,7 @@
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C112" s="2" t="s">
         <v>171</v>
       </c>
@@ -2494,7 +2479,7 @@
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>8</v>
       </c>
@@ -2502,102 +2487,91 @@
         <v>130</v>
       </c>
     </row>
-    <row r="118" spans="1:9" s="1" customFormat="1" ht="28.8">
-      <c r="C118" s="4" t="s">
+    <row r="118" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C118" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="D118" s="17" t="s">
+      <c r="D118" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="E118" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F118" s="5" t="s">
+      <c r="E118" s="14" t="s">
         <v>111</v>
       </c>
+      <c r="F118" s="15" t="s">
+        <v>112</v>
+      </c>
       <c r="G118" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="H118" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="I118" s="9" t="s">
+      <c r="H118" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
       <c r="G119" s="2"/>
       <c r="H119" s="2"/>
-      <c r="I119" s="2"/>
-    </row>
-    <row r="120" spans="1:9">
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
-      <c r="I120" s="2"/>
-    </row>
-    <row r="121" spans="1:9">
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
-      <c r="I121" s="2"/>
-    </row>
-    <row r="122" spans="1:9">
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
       <c r="G122" s="2"/>
       <c r="H122" s="2"/>
-      <c r="I122" s="2"/>
-    </row>
-    <row r="123" spans="1:9">
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
-      <c r="I123" s="2"/>
-    </row>
-    <row r="124" spans="1:9">
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
       <c r="G124" s="2"/>
       <c r="H124" s="2"/>
-      <c r="I124" s="2"/>
-    </row>
-    <row r="125" spans="1:9">
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
-      <c r="I125" s="2"/>
-    </row>
-    <row r="126" spans="1:9">
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
       <c r="F126" s="2"/>
       <c r="G126" s="2"/>
       <c r="H126" s="2"/>
-      <c r="I126" s="2"/>
-    </row>
-    <row r="131" spans="1:11">
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>9</v>
       </c>
@@ -2605,36 +2579,36 @@
         <v>133</v>
       </c>
     </row>
-    <row r="132" spans="1:11" s="1" customFormat="1" ht="43.2">
-      <c r="C132" s="4" t="s">
+    <row r="132" spans="1:11" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C132" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D132" s="4" t="s">
+      <c r="D132" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="E132" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F132" s="4" t="s">
+      <c r="E132" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F132" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G132" s="14" t="s">
+      <c r="G132" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="H132" s="14" t="s">
+      <c r="H132" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="I132" s="14" t="s">
+      <c r="I132" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="J132" s="14" t="s">
+      <c r="J132" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="K132" s="9" t="s">
+      <c r="K132" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:11">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C133" s="2" t="s">
         <v>139</v>
       </c>
@@ -2647,7 +2621,7 @@
       <c r="J133" s="2"/>
       <c r="K133" s="2"/>
     </row>
-    <row r="134" spans="1:11">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C134" s="2" t="s">
         <v>140</v>
       </c>
@@ -2660,7 +2634,7 @@
       <c r="J134" s="2"/>
       <c r="K134" s="2"/>
     </row>
-    <row r="135" spans="1:11">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C135" s="2" t="s">
         <v>141</v>
       </c>
@@ -2673,7 +2647,7 @@
       <c r="J135" s="2"/>
       <c r="K135" s="2"/>
     </row>
-    <row r="136" spans="1:11">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C136" s="2" t="s">
         <v>142</v>
       </c>
@@ -2686,7 +2660,7 @@
       <c r="J136" s="2"/>
       <c r="K136" s="2"/>
     </row>
-    <row r="137" spans="1:11">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C137" s="2" t="s">
         <v>143</v>
       </c>
@@ -2699,7 +2673,7 @@
       <c r="J137" s="2"/>
       <c r="K137" s="2"/>
     </row>
-    <row r="138" spans="1:11">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C138" s="2" t="s">
         <v>144</v>
       </c>
@@ -2712,7 +2686,7 @@
       <c r="J138" s="2"/>
       <c r="K138" s="2"/>
     </row>
-    <row r="139" spans="1:11">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C139" s="2" t="s">
         <v>145</v>
       </c>
@@ -2725,13 +2699,13 @@
       <c r="J139" s="2"/>
       <c r="K139" s="2"/>
     </row>
-    <row r="144" spans="1:11" ht="43.2">
-      <c r="E144" s="14" t="s">
+    <row r="144" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E144" s="11" t="s">
         <v>136</v>
       </c>
       <c r="F144" s="2"/>
     </row>
-    <row r="145" spans="1:11">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E145" s="2" t="s">
         <v>137</v>
       </c>
@@ -2739,7 +2713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:11">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E146" s="2" t="s">
         <v>138</v>
       </c>
@@ -2747,7 +2721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:11">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E147" s="2" t="s">
         <v>148</v>
       </c>
@@ -2755,7 +2729,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="152" spans="1:11">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>10</v>
       </c>
@@ -2763,36 +2737,36 @@
         <v>182</v>
       </c>
     </row>
-    <row r="153" spans="1:11" s="1" customFormat="1" ht="28.8">
-      <c r="C153" s="4" t="s">
+    <row r="153" spans="1:11" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C153" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="D153" s="5" t="s">
+      <c r="D153" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="E153" s="4" t="s">
+      <c r="E153" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="F153" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G153" s="5" t="s">
+      <c r="F153" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G153" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="H153" s="5" t="s">
+      <c r="H153" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="I153" s="14" t="s">
+      <c r="I153" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="J153" s="14" t="s">
+      <c r="J153" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="K153" s="9" t="s">
+      <c r="K153" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="154" spans="1:11">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C154" s="2" t="s">
         <v>156</v>
       </c>
@@ -2807,7 +2781,7 @@
       <c r="J154" s="2"/>
       <c r="K154" s="2"/>
     </row>
-    <row r="155" spans="1:11">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C155" s="2" t="s">
         <v>157</v>
       </c>
@@ -2822,7 +2796,7 @@
       <c r="J155" s="2"/>
       <c r="K155" s="2"/>
     </row>
-    <row r="156" spans="1:11">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C156" s="2" t="s">
         <v>158</v>
       </c>
@@ -2837,7 +2811,7 @@
       <c r="J156" s="2"/>
       <c r="K156" s="2"/>
     </row>
-    <row r="157" spans="1:11">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C157" s="2" t="s">
         <v>159</v>
       </c>
@@ -2852,7 +2826,7 @@
       <c r="J157" s="2"/>
       <c r="K157" s="2"/>
     </row>
-    <row r="158" spans="1:11">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C158" s="2" t="s">
         <v>160</v>
       </c>
@@ -2867,7 +2841,7 @@
       <c r="J158" s="2"/>
       <c r="K158" s="2"/>
     </row>
-    <row r="159" spans="1:11">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C159" s="2" t="s">
         <v>161</v>
       </c>

</xml_diff>

<commit_message>
Created resources\views\systemAdmin\users-table.blade.php to show users and esources\views\systemAdmin\SysAdmincomponent\create-new-user.blade.php to create a new user
</commit_message>
<xml_diff>
--- a/Documents/ER_Inventory/Test_Excel.xlsx
+++ b/Documents/ER_Inventory/Test_Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SALINDA SANDARUWAN\SIBA_Dynamics\SIBA-Inventory-system-Dynamics\Inventory-2k23\Documents\ER_Inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33EC674-8FDD-451A-89B3-7FDEA4EDF077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE709F5B-75B1-4387-8D65-2B9F37445E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{7C6AD97D-0354-4FD0-8E91-EBAC4EC551C4}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="184">
   <si>
     <t>state</t>
   </si>
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95CA8C8-82BE-40BC-8871-F9C457D45A7D}">
   <dimension ref="A2:T159"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A148" zoomScale="102" zoomScaleNormal="117" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B157" sqref="B157"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="102" zoomScaleNormal="117" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1128,9 +1128,6 @@
         <v>108</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="O3" s="14" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1151,7 +1148,6 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
@@ -1180,9 +1176,6 @@
       <c r="N5" s="2">
         <v>1</v>
       </c>
-      <c r="O5" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
@@ -1211,9 +1204,6 @@
       <c r="N6" s="2">
         <v>1</v>
       </c>
-      <c r="O6" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
@@ -1240,9 +1230,6 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2">
-        <v>0</v>
-      </c>
-      <c r="O7" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1273,9 +1260,6 @@
       <c r="N8" s="2">
         <v>1</v>
       </c>
-      <c r="O8" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="9" spans="1:16" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
@@ -1304,9 +1288,6 @@
       <c r="N9" s="2">
         <v>1</v>
       </c>
-      <c r="O9" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
@@ -1335,9 +1316,6 @@
       <c r="N10" s="2">
         <v>1</v>
       </c>
-      <c r="O10" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
@@ -1364,9 +1342,6 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2">
-        <v>1</v>
-      </c>
-      <c r="O11" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>